<commit_message>
minor updates and formatting
</commit_message>
<xml_diff>
--- a/front-and-back-matter/preface/attributions-blackrat.xlsx
+++ b/front-and-back-matter/preface/attributions-blackrat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Siobhon/Documents/Uni/PhD/Thesis-docs/PhD_thesis/front-and-back-matter/preface/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Siobhon/Documents/Uni/PhD/Thesis-docs/PhD/front-and-back-matter/preface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E0481B-6018-024A-B692-265FF7FC4F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422B6A48-7950-D440-B7AB-21AE20D8B96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="460" windowWidth="27560" windowHeight="17540" xr2:uid="{A1539C1E-5C51-ED44-AA70-CB3B0449F689}"/>
   </bookViews>
@@ -76,10 +76,10 @@
     <t>Liisa A. Ahlstrom</t>
   </si>
   <si>
-    <t>Draft</t>
-  </si>
-  <si>
     <t>Data Analysis</t>
+  </si>
+  <si>
+    <t>Drafting of manuscript</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,10 +467,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>